<commit_message>
feat: updated test excel file for warning cases
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383C293E-10D2-4BFE-A7CE-C40FC829595D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81DBF25-E8CD-44E0-9A71-810AEFB1B65C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="28800" windowHeight="17565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="91">
   <si>
     <t>Unique ID</t>
   </si>
@@ -256,9 +256,6 @@
     <t>èèèèèèèèèèèèèèèèèèèèèèèèèèèèèèèè</t>
   </si>
   <si>
-    <t>èèèèèèèèèèèèèèèèèèèèè</t>
-  </si>
-  <si>
     <t>èè</t>
   </si>
   <si>
@@ -266,6 +263,39 @@
   </si>
   <si>
     <t>./listing/{lang}.json</t>
+  </si>
+  <si>
+    <t>zerg</t>
+  </si>
+  <si>
+    <t>zreg</t>
+  </si>
+  <si>
+    <t>azer</t>
+  </si>
+  <si>
+    <t>wxcv</t>
+  </si>
+  <si>
+    <t>zge</t>
+  </si>
+  <si>
+    <t>rtyu</t>
+  </si>
+  <si>
+    <t>tryu</t>
+  </si>
+  <si>
+    <t>fhgj</t>
+  </si>
+  <si>
+    <t>rtyj</t>
+  </si>
+  <si>
+    <t>fghj</t>
+  </si>
+  <si>
+    <t>gfhj</t>
   </si>
 </sst>
 </file>
@@ -710,7 +740,7 @@
   <dimension ref="A1:F705"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -798,6 +828,9 @@
       <c r="D5" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="F5" s="5" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1">
       <c r="A6" s="12"/>
@@ -810,6 +843,9 @@
       <c r="D6" s="5" t="s">
         <v>52</v>
       </c>
+      <c r="F6" s="5" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="7" spans="1:6" s="5" customFormat="1">
       <c r="A7" s="12"/>
@@ -822,6 +858,9 @@
       <c r="D7" s="5" t="s">
         <v>53</v>
       </c>
+      <c r="F7" s="5" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="8" spans="1:6" s="5" customFormat="1">
       <c r="A8" s="12"/>
@@ -834,6 +873,9 @@
       <c r="D8" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="F8" s="5" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="9" spans="1:6" s="5" customFormat="1">
       <c r="A9" s="12"/>
@@ -864,6 +906,9 @@
       <c r="D10" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F10" s="5" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="11" spans="1:6" s="5" customFormat="1">
       <c r="A11" s="12"/>
@@ -879,6 +924,9 @@
       <c r="E11" s="5" t="s">
         <v>73</v>
       </c>
+      <c r="F11" s="5" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="12" spans="1:6" s="20" customFormat="1" ht="30" customHeight="1">
       <c r="A12" s="18" t="s">
@@ -902,7 +950,9 @@
       <c r="D13" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="5"/>
+      <c r="F13" s="5" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="B14" t="s">
@@ -915,7 +965,7 @@
         <v>4</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -928,7 +978,9 @@
       <c r="D15" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="5"/>
+      <c r="F15" s="5" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="16" spans="1:6" s="20" customFormat="1" ht="30" customHeight="1">
       <c r="A16" s="18" t="s">
@@ -947,7 +999,7 @@
         <v>28</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
@@ -968,7 +1020,7 @@
         <v>74</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -981,7 +1033,9 @@
       <c r="D19" t="s">
         <v>61</v>
       </c>
-      <c r="F19" s="5"/>
+      <c r="F19" s="5" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="20" spans="1:6">
       <c r="B20" t="s">
@@ -993,7 +1047,9 @@
       <c r="D20" t="s">
         <v>62</v>
       </c>
-      <c r="F20" s="5"/>
+      <c r="F20" s="5" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="21" spans="1:6">
       <c r="B21" t="s">
@@ -1005,7 +1061,9 @@
       <c r="D21" t="s">
         <v>63</v>
       </c>
-      <c r="F21" s="5"/>
+      <c r="F21" s="5" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="22" spans="1:6">
       <c r="B22" t="s">
@@ -1017,7 +1075,9 @@
       <c r="D22" t="s">
         <v>64</v>
       </c>
-      <c r="F22" s="5"/>
+      <c r="F22" s="5" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="23" spans="1:6">
       <c r="B23" t="s">
@@ -1030,7 +1090,7 @@
         <v>65</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1046,7 +1106,9 @@
       <c r="E24" t="s">
         <v>75</v>
       </c>
-      <c r="F24" s="5"/>
+      <c r="F24" s="5" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="25" spans="1:6">
       <c r="B25" t="s">
@@ -1070,7 +1132,9 @@
       <c r="D26" t="s">
         <v>18</v>
       </c>
-      <c r="F26" s="5"/>
+      <c r="F26" s="5" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="27" spans="1:6">
       <c r="B27" t="s">

</xml_diff>

<commit_message>
test: new excel file for duplicate tests
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81DBF25-E8CD-44E0-9A71-810AEFB1B65C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38807C70-BA1C-4A3B-B8DF-67161ED0D069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29340" yWindow="885" windowWidth="24900" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="92">
   <si>
     <t>Unique ID</t>
   </si>
@@ -296,6 +296,9 @@
   </si>
   <si>
     <t>gfhj</t>
+  </si>
+  <si>
+    <t>Save2</t>
   </si>
 </sst>
 </file>
@@ -740,7 +743,7 @@
   <dimension ref="A1:F705"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -982,173 +985,179 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="20" customFormat="1" ht="30" customHeight="1">
-      <c r="A16" s="18" t="s">
+    <row r="16" spans="1:6">
+      <c r="B16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" t="s">
+        <v>91</v>
+      </c>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" s="20" customFormat="1" ht="30" customHeight="1">
+      <c r="A17" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B17" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-    </row>
-    <row r="17" spans="1:6" s="14" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A17" s="15" t="s">
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+    </row>
+    <row r="18" spans="1:6" s="14" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A18" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B18" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="B18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" t="s">
-        <v>74</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>77</v>
-      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
     </row>
     <row r="19" spans="1:6">
       <c r="B19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="E19" t="s">
+        <v>74</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="B20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="B21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="B22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="D22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="B23" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="B24" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="C24" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="B25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D25" t="s">
-        <v>17</v>
-      </c>
-      <c r="F25" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="E25" t="s">
+        <v>75</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="26" spans="1:6">
       <c r="B26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D26" t="s">
-        <v>18</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>88</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6">
       <c r="B27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="B28" t="s">
         <v>41</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>59</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>59</v>
       </c>
-      <c r="F27" s="5"/>
-    </row>
-    <row r="28" spans="1:6">
       <c r="F28" s="5"/>
     </row>
     <row r="29" spans="1:6">

</xml_diff>